<commit_message>
Added white tile in excel
</commit_message>
<xml_diff>
--- a/TileMifs.xlsx
+++ b/TileMifs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="21040" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="80">
   <si>
     <t>000</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Table Map</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -304,8 +307,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -346,7 +355,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +372,9 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -379,6 +391,9 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -708,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV54"/>
+  <dimension ref="A1:AV59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP8" workbookViewId="0">
-      <selection activeCell="AU43" sqref="AU43"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42:AK59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2889,11 +2904,119 @@
       </c>
     </row>
     <row r="42" spans="20:43">
+      <c r="T42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK42" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN42" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="43" spans="20:43">
+      <c r="T43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK43" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN43" s="1" t="s">
         <v>25</v>
       </c>
@@ -2902,6 +3025,60 @@
       </c>
     </row>
     <row r="44" spans="20:43">
+      <c r="T44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK44" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN44" s="1" t="s">
         <v>26</v>
       </c>
@@ -2910,6 +3087,60 @@
       </c>
     </row>
     <row r="45" spans="20:43">
+      <c r="T45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK45" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN45" s="1" t="s">
         <v>27</v>
       </c>
@@ -2921,6 +3152,60 @@
       </c>
     </row>
     <row r="46" spans="20:43">
+      <c r="T46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK46" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN46" s="1" t="s">
         <v>28</v>
       </c>
@@ -2935,6 +3220,60 @@
       </c>
     </row>
     <row r="47" spans="20:43">
+      <c r="T47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK47" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN47" s="1" t="s">
         <v>29</v>
       </c>
@@ -2946,6 +3285,60 @@
       </c>
     </row>
     <row r="48" spans="20:43">
+      <c r="T48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK48" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN48" s="1" t="s">
         <v>30</v>
       </c>
@@ -2956,7 +3349,61 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="40:43">
+    <row r="49" spans="20:43">
+      <c r="T49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK49" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN49" s="1" t="s">
         <v>31</v>
       </c>
@@ -2967,7 +3414,61 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="40:43">
+    <row r="50" spans="20:43">
+      <c r="T50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK50" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN50" s="1" t="s">
         <v>32</v>
       </c>
@@ -2978,7 +3479,61 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="40:43">
+    <row r="51" spans="20:43">
+      <c r="T51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK51" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN51" s="1" t="s">
         <v>33</v>
       </c>
@@ -2989,7 +3544,61 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="40:43">
+    <row r="52" spans="20:43">
+      <c r="T52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK52" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN52" s="1" t="s">
         <v>34</v>
       </c>
@@ -2997,7 +3606,61 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="40:43">
+    <row r="53" spans="20:43">
+      <c r="T53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK53" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN53" s="1" t="s">
         <v>35</v>
       </c>
@@ -3005,12 +3668,346 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="40:43">
+    <row r="54" spans="20:43">
+      <c r="T54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK54" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AN54" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AO54" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="20:43">
+      <c r="T55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="20:43">
+      <c r="T56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="20:43">
+      <c r="T57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="20:43">
+      <c r="T58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK58" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="20:43">
+      <c r="T59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK59" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>